<commit_message>
upload drone city datasets
</commit_message>
<xml_diff>
--- a/data/ave-pm-2.5/ave-pm2.5-annual.xlsx
+++ b/data/ave-pm-2.5/ave-pm2.5-annual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\GitHub\ethno-urban-profile\data\ave-pm-2.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C230223F-8395-47A1-9CAB-14521941A0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9214A561-6C9C-48FE-82A8-A524912124F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="1632" windowWidth="17280" windowHeight="8952" xr2:uid="{5ED686D2-8303-466F-B5AE-935171263170}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5ED686D2-8303-466F-B5AE-935171263170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>